<commit_message>
office hours with murodil🙂
</commit_message>
<xml_diff>
--- a/VyTrackQa2Users.xlsx
+++ b/VyTrackQa2Users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Murodil/Downloads/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>username</t>
   </si>
@@ -190,12 +190,19 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -580,7 +587,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -597,7 +604,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -614,7 +621,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -631,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -648,7 +655,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -665,7 +672,7 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -682,7 +689,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -699,7 +706,7 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -716,7 +723,7 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -733,7 +740,7 @@
         <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -750,7 +757,7 @@
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -767,7 +774,7 @@
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -784,7 +791,7 @@
         <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -801,7 +808,7 @@
         <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -818,7 +825,7 @@
         <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>